<commit_message>
feat: support write Excel refactor: abstract method test: update
</commit_message>
<xml_diff>
--- a/excelflow-core/src/test/resources/excel/test1.xlsx
+++ b/excelflow-core/src/test/resources/excel/test1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bitWorkspace\ExcelPort\ExcelPort-Core\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\excelflow\excelflow-core\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECDCDD6-E616-491C-BC63-ED98FA2B8C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B030B-7F52-495C-99BC-20E12E9E7E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="810" windowWidth="21600" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38295" yWindow="825" windowWidth="16095" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,8 +225,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -510,7 +511,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A31" sqref="A31:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -736,6 +737,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -768,9 +772,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1153,6 +1155,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -1185,9 +1190,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -1220,6 +1223,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -1357,7 +1361,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -1392,6 +1396,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -1424,7 +1429,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1459,6 +1464,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>44</v>
       </c>
@@ -1491,7 +1497,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1526,6 +1532,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>46</v>
       </c>
@@ -1558,7 +1565,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1593,6 +1600,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>48</v>
       </c>
@@ -1624,7 +1632,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
       <c r="B33" t="s">
         <v>49</v>
       </c>
@@ -1657,6 +1666,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>